<commit_message>
Se agregó una nueva clase
</commit_message>
<xml_diff>
--- a/Trabajo de analisis.xlsx
+++ b/Trabajo de analisis.xlsx
@@ -5,27 +5,39 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC10\Downloads\numeroPerfecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC19\Downloads\numeroPerfecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D98E438-6947-4531-8482-C42F8DDBEE53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEFD370-E715-490F-8D6E-05F6F21C07B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{304ACAD7-2492-4B24-AB01-9B5FF1E8D717}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{304ACAD7-2492-4B24-AB01-9B5FF1E8D717}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Numero Perfecto" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz Random" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
   <si>
     <t>Valor</t>
   </si>
@@ -155,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -168,17 +180,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -313,7 +323,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$11</c:f>
+              <c:f>'Numero Perfecto'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -352,7 +362,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$2:$G$11</c:f>
+              <c:f>'Numero Perfecto'!$G$2:$G$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -659,7 +669,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$16:$A$25</c:f>
+              <c:f>'Numero Perfecto'!$A$16:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -698,7 +708,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$16:$G$25</c:f>
+              <c:f>'Numero Perfecto'!$G$16:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1005,7 +1015,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$33:$A$42</c:f>
+              <c:f>'Numero Perfecto'!$A$33:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1044,7 +1054,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$33:$G$42</c:f>
+              <c:f>'Numero Perfecto'!$G$33:$G$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1259,6 +1269,352 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-CO"/>
+              <a:t>Promedio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CO"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Matriz Random'!$A$2:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Matriz Random'!$G$2:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10028980</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9738720</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12012940</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13517780</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17026640</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21566160</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27556800</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39369480</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43229740</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68223340</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CE0-45E3-94AF-D578B5C73738}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="419667615"/>
+        <c:axId val="419664255"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="419667615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419664255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="419664255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419667615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CO"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1379,6 +1735,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2386,6 +2782,522 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3016,6 +3928,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19D590EF-B38E-2A7F-9E39-BB28BCA207EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B4B7765F-7E73-4F3D-8A1E-E1F982B876D9}" name="Tabla1" displayName="Tabla1" ref="A1:G11" totalsRowShown="0">
   <autoFilter ref="A1:G11" xr:uid="{B4B7765F-7E73-4F3D-8A1E-E1F982B876D9}"/>
@@ -3029,7 +3982,7 @@
     <tableColumn id="4" xr3:uid="{B6762C6B-9BD9-43DE-9292-5A7945B5BD54}" name="T3"/>
     <tableColumn id="5" xr3:uid="{0CD3BDF0-33A0-4649-A9A8-B2480A440D39}" name="T4"/>
     <tableColumn id="6" xr3:uid="{41873EEF-7D12-4609-AB29-20815DFCB2AF}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{5B8074DC-C11E-47A8-801C-40B5E4101C66}" name="Promo" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{5B8074DC-C11E-47A8-801C-40B5E4101C66}" name="Promo" dataDxfId="3">
       <calculatedColumnFormula>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3050,7 +4003,7 @@
     <tableColumn id="4" xr3:uid="{B1E1AEFE-F461-4D1E-8583-732148F181AE}" name="T3"/>
     <tableColumn id="5" xr3:uid="{3E169A64-2E9E-4FBC-88A6-2B3A5DA975A5}" name="T4"/>
     <tableColumn id="6" xr3:uid="{5A38A4FF-1F31-44E6-91B7-814934850F20}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{15768844-E1EC-4756-9046-244EF02EA29A}" name="Promo" dataDxfId="1">
+    <tableColumn id="7" xr3:uid="{15768844-E1EC-4756-9046-244EF02EA29A}" name="Promo" dataDxfId="2">
       <calculatedColumnFormula>(Tabla13[[#This Row],[T1]]+Tabla13[[#This Row],[T2]]+Tabla13[[#This Row],[T3]]+Tabla13[[#This Row],[T4]]+Tabla13[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3071,8 +4024,29 @@
     <tableColumn id="4" xr3:uid="{AFB17FAC-4849-4874-B603-73AA4CBECAA9}" name="T3"/>
     <tableColumn id="5" xr3:uid="{B19C4136-67BC-48DE-8A6E-D6DC5A82B2EB}" name="T4"/>
     <tableColumn id="6" xr3:uid="{3DA0D3EA-B620-451E-8EEA-BFFB6BE91DBB}" name="T5"/>
-    <tableColumn id="7" xr3:uid="{4075EDF8-CE19-49EF-9147-3C602DBEF8D5}" name="Promo" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{4075EDF8-CE19-49EF-9147-3C602DBEF8D5}" name="Promo" dataDxfId="1">
       <calculatedColumnFormula>(Tabla134[[#This Row],[T1]]+Tabla134[[#This Row],[T2]]+Tabla134[[#This Row],[T3]]+Tabla134[[#This Row],[T4]]+Tabla134[[#This Row],[T5]])/5</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3E9D5BA6-E2F2-4DC2-9745-7746D1D7B151}" name="Tabla1345" displayName="Tabla1345" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11" xr:uid="{3E9D5BA6-E2F2-4DC2-9745-7746D1D7B151}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G11">
+    <sortCondition descending="1" ref="A16:A25"/>
+  </sortState>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{11793D7E-5304-4E5D-9237-1DAF65E37084}" name="Valor"/>
+    <tableColumn id="2" xr3:uid="{EF1FA859-5B76-47DF-A561-E3CDD3F513CE}" name="T1"/>
+    <tableColumn id="3" xr3:uid="{BFBB43F9-DC8A-4335-AFA6-8ED5FB02955F}" name="T2"/>
+    <tableColumn id="4" xr3:uid="{FEABBAAF-E83A-415D-9CFA-29F2F46FCFB9}" name="T3"/>
+    <tableColumn id="5" xr3:uid="{1A7250B2-518A-4296-A335-15549158DF19}" name="T4"/>
+    <tableColumn id="6" xr3:uid="{51CABBB4-62DB-461C-96BB-60847DA8D501}" name="T5"/>
+    <tableColumn id="7" xr3:uid="{D62087F7-8268-4318-8C12-FF090C078993}" name="Promo" dataDxfId="0">
+      <calculatedColumnFormula>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -3378,8 +4352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1B845E-1BE4-4F60-B45B-737BD01267B9}">
   <dimension ref="A1:N42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3437,7 +4411,7 @@
       <c r="F2" s="3">
         <v>78000</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="3">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>94240</v>
       </c>
@@ -3467,7 +4441,7 @@
       <c r="F3">
         <v>9400</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>9380</v>
       </c>
@@ -3499,7 +4473,7 @@
       <c r="F4">
         <v>6600</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>6880</v>
       </c>
@@ -3531,7 +4505,7 @@
       <c r="F5" s="2">
         <v>5700</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="2">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>11720</v>
       </c>
@@ -3563,7 +4537,7 @@
       <c r="F6">
         <v>1300</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>1360</v>
       </c>
@@ -3587,7 +4561,7 @@
       <c r="F7">
         <v>1100</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>1100</v>
       </c>
@@ -3611,7 +4585,7 @@
       <c r="F8">
         <v>800</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>740</v>
       </c>
@@ -3635,7 +4609,7 @@
       <c r="F9">
         <v>500</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>580</v>
       </c>
@@ -3659,7 +4633,7 @@
       <c r="F10">
         <v>500</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>520</v>
       </c>
@@ -3683,7 +4657,7 @@
       <c r="F11">
         <v>200</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11">
         <f>(Tabla1[[#This Row],[T1]]+Tabla1[[#This Row],[T2]]+Tabla1[[#This Row],[T3]]+Tabla1[[#This Row],[T4]]+Tabla1[[#This Row],[T5]])/5</f>
         <v>240</v>
       </c>
@@ -4231,4 +5205,287 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6422C6C1-1A07-4795-83A5-A536D9CCAFBC}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10357600</v>
+      </c>
+      <c r="C2" s="3">
+        <v>8305300</v>
+      </c>
+      <c r="D2" s="3">
+        <v>8773500</v>
+      </c>
+      <c r="E2" s="3">
+        <v>11769500</v>
+      </c>
+      <c r="F2" s="3">
+        <v>10939000</v>
+      </c>
+      <c r="G2" s="3">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>10028980</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>9155400</v>
+      </c>
+      <c r="C3">
+        <v>9818900</v>
+      </c>
+      <c r="D3">
+        <v>10547500</v>
+      </c>
+      <c r="E3">
+        <v>9917900</v>
+      </c>
+      <c r="F3">
+        <v>9253900</v>
+      </c>
+      <c r="G3">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>9738720</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>12383200</v>
+      </c>
+      <c r="C4">
+        <v>11334700</v>
+      </c>
+      <c r="D4">
+        <v>11986300</v>
+      </c>
+      <c r="E4">
+        <v>11549100</v>
+      </c>
+      <c r="F4">
+        <v>12811400</v>
+      </c>
+      <c r="G4">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>12012940</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13221800</v>
+      </c>
+      <c r="C5" s="2">
+        <v>12386100</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13430700</v>
+      </c>
+      <c r="E5" s="2">
+        <v>13570400</v>
+      </c>
+      <c r="F5" s="2">
+        <v>14979900</v>
+      </c>
+      <c r="G5" s="2">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>13517780</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>17197000</v>
+      </c>
+      <c r="C6">
+        <v>17313500</v>
+      </c>
+      <c r="D6">
+        <v>17092100</v>
+      </c>
+      <c r="E6">
+        <v>17208000</v>
+      </c>
+      <c r="F6">
+        <v>16322600</v>
+      </c>
+      <c r="G6">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>17026640</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>22286800</v>
+      </c>
+      <c r="C7">
+        <v>24882000</v>
+      </c>
+      <c r="D7">
+        <v>20482100</v>
+      </c>
+      <c r="E7">
+        <v>19664900</v>
+      </c>
+      <c r="F7">
+        <v>20515000</v>
+      </c>
+      <c r="G7">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>21566160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>25066800</v>
+      </c>
+      <c r="C8">
+        <v>28011100</v>
+      </c>
+      <c r="D8">
+        <v>27691400</v>
+      </c>
+      <c r="E8">
+        <v>26567500</v>
+      </c>
+      <c r="F8">
+        <v>30447200</v>
+      </c>
+      <c r="G8">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>27556800</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>45796600</v>
+      </c>
+      <c r="C9">
+        <v>35143900</v>
+      </c>
+      <c r="D9">
+        <v>36374000</v>
+      </c>
+      <c r="E9">
+        <v>38802300</v>
+      </c>
+      <c r="F9">
+        <v>40730600</v>
+      </c>
+      <c r="G9">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>39369480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>42438100</v>
+      </c>
+      <c r="C10">
+        <v>40543500</v>
+      </c>
+      <c r="D10">
+        <v>48997200</v>
+      </c>
+      <c r="E10">
+        <v>42737100</v>
+      </c>
+      <c r="F10">
+        <v>41432800</v>
+      </c>
+      <c r="G10">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>43229740</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>58072000</v>
+      </c>
+      <c r="C11">
+        <v>66227800</v>
+      </c>
+      <c r="D11">
+        <v>85806400</v>
+      </c>
+      <c r="E11">
+        <v>65343500</v>
+      </c>
+      <c r="F11">
+        <v>65667000</v>
+      </c>
+      <c r="G11">
+        <f>(Tabla1345[[#This Row],[T1]]+Tabla1345[[#This Row],[T2]]+Tabla1345[[#This Row],[T3]]+Tabla1345[[#This Row],[T4]]+Tabla1345[[#This Row],[T5]])/5</f>
+        <v>68223340</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>